<commit_message>
Process serialnumber is 4 digits
</commit_message>
<xml_diff>
--- a/barcodes.xlsx
+++ b/barcodes.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Customer ID</t>
   </si>
@@ -51,12 +51,6 @@
   </si>
   <si>
     <t>ft000540</t>
-  </si>
-  <si>
-    <t>00185</t>
-  </si>
-  <si>
-    <t>00189</t>
   </si>
   <si>
     <r>
@@ -83,12 +77,6 @@
   </si>
   <si>
     <t>xy987654</t>
-  </si>
-  <si>
-    <t>00190</t>
-  </si>
-  <si>
-    <t>00195</t>
   </si>
   <si>
     <r>
@@ -759,7 +747,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1102,7 +1090,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="6"/>
@@ -1146,35 +1134,35 @@
       <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="5">
+        <v>185</v>
+      </c>
+      <c r="E2" s="5">
+        <v>189</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="G2" s="2"/>
     </row>
     <row r="3" ht="13.9" spans="1:7">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3">
         <v>2034</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
+      </c>
+      <c r="D3" s="5">
+        <v>190</v>
+      </c>
+      <c r="E3" s="5">
+        <v>195</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G3" s="2"/>
     </row>

</xml_diff>